<commit_message>
dar de alta alumnos + solicitar correo con link de cambio de contraseña + cambio de contraseña
</commit_message>
<xml_diff>
--- a/src/assets/EjemploListaExcel.xlsx
+++ b/src/assets/EjemploListaExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E8C53A-ED3C-42E6-94FD-E46EA673AFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F17638-D620-4E85-A208-03E4C5799018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{2E99FCAF-7A53-9648-848D-EB83D1609C1D}"/>
+    <workbookView xWindow="4110" yWindow="2880" windowWidth="21600" windowHeight="11295" xr2:uid="{2E99FCAF-7A53-9648-848D-EB83D1609C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>LISTADO DE ALUMNOS MATRICULADOS</t>
   </si>
@@ -189,13 +189,22 @@
   </si>
   <si>
     <t>Evaluación Diferenciada</t>
+  </si>
+  <si>
+    <t>Gallego Doncel, Aljenadro</t>
+  </si>
+  <si>
+    <t>80239121X</t>
+  </si>
+  <si>
+    <t>UO285577@uniovi.es</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,6 +232,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,7 +249,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -255,11 +272,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,11 +297,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682D537C-4220-F243-AED1-2A7C1117AEA9}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1256,15 +1288,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1578,10 +1610,51 @@
         <v>29</v>
       </c>
     </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D18" r:id="rId1" xr:uid="{9B1D21B1-D397-41E6-AB60-ADF558F1612F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Notificación ene l cambio de grupo y en los alumnos desmatriculados
</commit_message>
<xml_diff>
--- a/src/assets/EjemploListaExcel.xlsx
+++ b/src/assets/EjemploListaExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F17638-D620-4E85-A208-03E4C5799018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF3A8AE-F28F-4DBF-A69C-D303D4085ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="2880" windowWidth="21600" windowHeight="11295" xr2:uid="{2E99FCAF-7A53-9648-848D-EB83D1609C1D}"/>
+    <workbookView xWindow="3975" yWindow="2955" windowWidth="21600" windowHeight="11295" xr2:uid="{2E99FCAF-7A53-9648-848D-EB83D1609C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>LISTADO DE ALUMNOS MATRICULADOS</t>
   </si>
@@ -171,21 +171,6 @@
   </si>
   <si>
     <t>UO567234@uniovi.es</t>
-  </si>
-  <si>
-    <t>Prácticas de Laboratorio-02</t>
-  </si>
-  <si>
-    <t>Tutorías Grupales-02</t>
-  </si>
-  <si>
-    <t>12345671K</t>
-  </si>
-  <si>
-    <t>Morales Fernández, María</t>
-  </si>
-  <si>
-    <t>UO654321@uniovi.es</t>
   </si>
   <si>
     <t>Evaluación Diferenciada</t>
@@ -298,10 +283,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -637,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682D537C-4220-F243-AED1-2A7C1117AEA9}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L17" sqref="I17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1288,15 +1273,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1342,7 +1327,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>13</v>
@@ -1563,88 +1548,50 @@
         <v>26</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="4">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
         <v>1</v>
       </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>8</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="4">
-        <v>2</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1653,7 +1600,7 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D18" r:id="rId1" xr:uid="{9B1D21B1-D397-41E6-AB60-ADF558F1612F}"/>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{9B1D21B1-D397-41E6-AB60-ADF558F1612F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reorganización de las tablas grupo-clases
</commit_message>
<xml_diff>
--- a/src/assets/EjemploListaExcel.xlsx
+++ b/src/assets/EjemploListaExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF3A8AE-F28F-4DBF-A69C-D303D4085ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D0012E-EA15-4138-A418-443831458CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="2955" windowWidth="21600" windowHeight="11295" xr2:uid="{2E99FCAF-7A53-9648-848D-EB83D1609C1D}"/>
+    <workbookView xWindow="1905" yWindow="3855" windowWidth="25935" windowHeight="11295" xr2:uid="{2E99FCAF-7A53-9648-848D-EB83D1609C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>LISTADO DE ALUMNOS MATRICULADOS</t>
   </si>
@@ -174,15 +174,6 @@
   </si>
   <si>
     <t>Evaluación Diferenciada</t>
-  </si>
-  <si>
-    <t>Gallego Doncel, Aljenadro</t>
-  </si>
-  <si>
-    <t>80239121X</t>
-  </si>
-  <si>
-    <t>UO285577@uniovi.es</t>
   </si>
 </sst>
 </file>
@@ -624,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682D537C-4220-F243-AED1-2A7C1117AEA9}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L17" sqref="I17:L17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1548,60 +1539,33 @@
         <v>26</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>8</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="4">
-        <v>2</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D17" r:id="rId1" xr:uid="{9B1D21B1-D397-41E6-AB60-ADF558F1612F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tablón de anuncios en pruebas
</commit_message>
<xml_diff>
--- a/src/assets/EjemploListaExcel.xlsx
+++ b/src/assets/EjemploListaExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D0012E-EA15-4138-A418-443831458CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE38533B-BF68-42A5-A0C8-508D5D764C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1905" yWindow="3855" windowWidth="25935" windowHeight="11295" xr2:uid="{2E99FCAF-7A53-9648-848D-EB83D1609C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>LISTADO DE ALUMNOS MATRICULADOS</t>
   </si>
@@ -174,6 +174,18 @@
   </si>
   <si>
     <t>Evaluación Diferenciada</t>
+  </si>
+  <si>
+    <t>80239121X</t>
+  </si>
+  <si>
+    <t>Gallego Doncel, Alejandro</t>
+  </si>
+  <si>
+    <t>UO285577@uniovi.es</t>
+  </si>
+  <si>
+    <t>Tutorías Grupales-02</t>
   </si>
 </sst>
 </file>
@@ -616,7 +628,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1549,23 +1561,50 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="A17" s="4">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{55E30194-41DF-40BB-BABA-0A0C7B0DFBC1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>